<commit_message>
nltk sentence length edit
</commit_message>
<xml_diff>
--- a/Data/all_inference.xlsx
+++ b/Data/all_inference.xlsx
@@ -18932,13 +18932,17 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D478" t="inlineStr"/>
-      <c r="E478" t="inlineStr"/>
+      <c r="D478" t="n">
+        <v>-28.83124167177692</v>
+      </c>
+      <c r="E478" t="n">
+        <v>5.826759107556711e-50</v>
+      </c>
       <c r="F478" t="inlineStr"/>
       <c r="G478" t="inlineStr"/>
       <c r="H478" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I478" t="inlineStr">
@@ -18947,10 +18951,10 @@
         </is>
       </c>
       <c r="J478" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K478" t="n">
-        <v>0</v>
+        <v>10.77</v>
       </c>
     </row>
     <row r="479">
@@ -18969,13 +18973,17 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D479" t="inlineStr"/>
-      <c r="E479" t="inlineStr"/>
+      <c r="D479" t="n">
+        <v>-35.07760175955924</v>
+      </c>
+      <c r="E479" t="n">
+        <v>1.207408057620094e-57</v>
+      </c>
       <c r="F479" t="inlineStr"/>
       <c r="G479" t="inlineStr"/>
       <c r="H479" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I479" t="inlineStr">
@@ -18984,10 +18992,10 @@
         </is>
       </c>
       <c r="J479" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K479" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="480">
@@ -19006,13 +19014,17 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D480" t="inlineStr"/>
-      <c r="E480" t="inlineStr"/>
+      <c r="D480" t="n">
+        <v>-6.363129794846619</v>
+      </c>
+      <c r="E480" t="n">
+        <v>6.177619637446933e-09</v>
+      </c>
       <c r="F480" t="inlineStr"/>
       <c r="G480" t="inlineStr"/>
       <c r="H480" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I480" t="inlineStr">
@@ -19021,10 +19033,10 @@
         </is>
       </c>
       <c r="J480" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K480" t="n">
-        <v>0</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="481">
@@ -19043,13 +19055,17 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D481" t="inlineStr"/>
-      <c r="E481" t="inlineStr"/>
+      <c r="D481" t="n">
+        <v>2.148395723904016</v>
+      </c>
+      <c r="E481" t="n">
+        <v>0.03412159030060466</v>
+      </c>
       <c r="F481" t="inlineStr"/>
       <c r="G481" t="inlineStr"/>
       <c r="H481" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I481" t="inlineStr">
@@ -19058,10 +19074,10 @@
         </is>
       </c>
       <c r="J481" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K481" t="n">
-        <v>0</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="482">
@@ -19072,7 +19088,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
@@ -19080,13 +19096,17 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D482" t="inlineStr"/>
-      <c r="E482" t="inlineStr"/>
+      <c r="D482" t="n">
+        <v>-9.692851718495611</v>
+      </c>
+      <c r="E482" t="n">
+        <v>5.118579912527966e-16</v>
+      </c>
       <c r="F482" t="inlineStr"/>
       <c r="G482" t="inlineStr"/>
       <c r="H482" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I482" t="inlineStr">
@@ -19095,10 +19115,10 @@
         </is>
       </c>
       <c r="J482" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K482" t="n">
-        <v>0</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="483">
@@ -19109,7 +19129,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
@@ -19118,10 +19138,10 @@
         </is>
       </c>
       <c r="D483" t="n">
-        <v>-17.28490257834441</v>
+        <v>-31.80941414812338</v>
       </c>
       <c r="E483" t="n">
-        <v>1.164213909357614e-31</v>
+        <v>8.853010573051538e-54</v>
       </c>
       <c r="F483" t="inlineStr"/>
       <c r="G483" t="inlineStr"/>
@@ -19136,10 +19156,10 @@
         </is>
       </c>
       <c r="J483" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K483" t="n">
-        <v>1.56</v>
+        <v>18.54</v>
       </c>
     </row>
     <row r="484">
@@ -19150,7 +19170,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
@@ -19158,13 +19178,11 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D484" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+      <c r="D484" t="n">
+        <v>-36.98836236107769</v>
       </c>
       <c r="E484" t="n">
-        <v>0</v>
+        <v>9.151685699063212e-60</v>
       </c>
       <c r="F484" t="inlineStr"/>
       <c r="G484" t="inlineStr"/>
@@ -19179,10 +19197,10 @@
         </is>
       </c>
       <c r="J484" t="n">
-        <v>0</v>
+        <v>2.08</v>
       </c>
       <c r="K484" t="n">
-        <v>4</v>
+        <v>10.93</v>
       </c>
     </row>
     <row r="485">
@@ -19193,7 +19211,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>ape_zero_shot_cot</t>
+          <t>manual_cot</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
@@ -19201,8 +19219,12 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D485" t="inlineStr"/>
-      <c r="E485" t="inlineStr"/>
+      <c r="D485" t="n">
+        <v>0.9039913210172316</v>
+      </c>
+      <c r="E485" t="n">
+        <v>0.3681945108696839</v>
+      </c>
       <c r="F485" t="inlineStr"/>
       <c r="G485" t="inlineStr"/>
       <c r="H485" t="inlineStr">
@@ -19216,10 +19238,10 @@
         </is>
       </c>
       <c r="J485" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K485" t="n">
-        <v>0</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="486">
@@ -19230,7 +19252,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>least_to_most</t>
+          <t>ape_zero_shot_cot</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
@@ -19238,13 +19260,17 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D486" t="inlineStr"/>
-      <c r="E486" t="inlineStr"/>
+      <c r="D486" t="n">
+        <v>-10.49397901206296</v>
+      </c>
+      <c r="E486" t="n">
+        <v>9.172631925799708e-18</v>
+      </c>
       <c r="F486" t="inlineStr"/>
       <c r="G486" t="inlineStr"/>
       <c r="H486" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I486" t="inlineStr">
@@ -19253,10 +19279,10 @@
         </is>
       </c>
       <c r="J486" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K486" t="n">
-        <v>0</v>
+        <v>4.64</v>
       </c>
     </row>
     <row r="487">
@@ -19267,7 +19293,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>manual_cot</t>
+          <t>least_to_most</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
@@ -19275,13 +19301,17 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D487" t="inlineStr"/>
-      <c r="E487" t="inlineStr"/>
+      <c r="D487" t="n">
+        <v>-24.03014668134204</v>
+      </c>
+      <c r="E487" t="n">
+        <v>4.207193365810621e-43</v>
+      </c>
       <c r="F487" t="inlineStr"/>
       <c r="G487" t="inlineStr"/>
       <c r="H487" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I487" t="inlineStr">
@@ -19290,10 +19320,10 @@
         </is>
       </c>
       <c r="J487" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K487" t="n">
-        <v>0</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="488">
@@ -19312,13 +19342,17 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D488" t="inlineStr"/>
-      <c r="E488" t="inlineStr"/>
+      <c r="D488" t="n">
+        <v>7.743797601653323</v>
+      </c>
+      <c r="E488" t="n">
+        <v>8.457009230169744e-12</v>
+      </c>
       <c r="F488" t="inlineStr"/>
       <c r="G488" t="inlineStr"/>
       <c r="H488" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I488" t="inlineStr">
@@ -19327,7 +19361,7 @@
         </is>
       </c>
       <c r="J488" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K488" t="n">
         <v>0</v>
@@ -19341,7 +19375,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
@@ -19349,13 +19383,17 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D489" t="inlineStr"/>
-      <c r="E489" t="inlineStr"/>
+      <c r="D489" t="n">
+        <v>-11.09174311926606</v>
+      </c>
+      <c r="E489" t="n">
+        <v>4.620740408183364e-19</v>
+      </c>
       <c r="F489" t="inlineStr"/>
       <c r="G489" t="inlineStr"/>
       <c r="H489" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I489" t="inlineStr">
@@ -19364,10 +19402,10 @@
         </is>
       </c>
       <c r="J489" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K489" t="n">
-        <v>0</v>
+        <v>5.37</v>
       </c>
     </row>
     <row r="490">
@@ -19378,7 +19416,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
@@ -19387,10 +19425,10 @@
         </is>
       </c>
       <c r="D490" t="n">
-        <v>-22.34110561274889</v>
+        <v>-23.81588001701261</v>
       </c>
       <c r="E490" t="n">
-        <v>1.880219793050742e-40</v>
+        <v>8.971196615459257e-43</v>
       </c>
       <c r="F490" t="inlineStr"/>
       <c r="G490" t="inlineStr"/>
@@ -19405,10 +19443,10 @@
         </is>
       </c>
       <c r="J490" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K490" t="n">
-        <v>2.2</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="491">
@@ -19419,7 +19457,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
@@ -19428,10 +19466,10 @@
         </is>
       </c>
       <c r="D491" t="n">
-        <v>-19.88471453556187</v>
+        <v>-7.439660703593491</v>
       </c>
       <c r="E491" t="n">
-        <v>2.38480654894213e-36</v>
+        <v>3.727399370914456e-11</v>
       </c>
       <c r="F491" t="inlineStr"/>
       <c r="G491" t="inlineStr"/>
@@ -19446,10 +19484,10 @@
         </is>
       </c>
       <c r="J491" t="n">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="K491" t="n">
-        <v>5.11</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="492">
@@ -20071,7 +20109,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>least_to_most</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
@@ -20108,7 +20146,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>manual_cot</t>
+          <t>least_to_most</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -20116,13 +20154,19 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D508" t="inlineStr"/>
-      <c r="E508" t="inlineStr"/>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E508" t="n">
+        <v>0</v>
+      </c>
       <c r="F508" t="inlineStr"/>
       <c r="G508" t="inlineStr"/>
       <c r="H508" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I508" t="inlineStr">
@@ -20134,7 +20178,7 @@
         <v>0</v>
       </c>
       <c r="K508" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="509">
@@ -20145,7 +20189,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>manual_few_shot</t>
+          <t>manual_cot</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
@@ -20153,13 +20197,19 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D509" t="inlineStr"/>
-      <c r="E509" t="inlineStr"/>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E509" t="n">
+        <v>0</v>
+      </c>
       <c r="F509" t="inlineStr"/>
       <c r="G509" t="inlineStr"/>
       <c r="H509" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I509" t="inlineStr">
@@ -20171,7 +20221,7 @@
         <v>0</v>
       </c>
       <c r="K509" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="510">
@@ -20182,7 +20232,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>manual_few_shot</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
@@ -20190,13 +20240,19 @@
           <t>cw</t>
         </is>
       </c>
-      <c r="D510" t="inlineStr"/>
-      <c r="E510" t="inlineStr"/>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E510" t="n">
+        <v>0</v>
+      </c>
       <c r="F510" t="inlineStr"/>
       <c r="G510" t="inlineStr"/>
       <c r="H510" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I510" t="inlineStr">
@@ -20208,7 +20264,7 @@
         <v>0</v>
       </c>
       <c r="K510" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="511">
@@ -20228,10 +20284,10 @@
         </is>
       </c>
       <c r="D511" t="n">
-        <v>-17.28490257834441</v>
+        <v>-22.8249354560189</v>
       </c>
       <c r="E511" t="n">
-        <v>1.164213909357614e-31</v>
+        <v>3.171891628034546e-41</v>
       </c>
       <c r="F511" t="inlineStr"/>
       <c r="G511" t="inlineStr"/>
@@ -20249,7 +20305,7 @@
         <v>0</v>
       </c>
       <c r="K511" t="n">
-        <v>1.56</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="512">
@@ -20292,7 +20348,7 @@
         <v>0</v>
       </c>
       <c r="K512" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="513">
@@ -20311,13 +20367,19 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D513" t="inlineStr"/>
-      <c r="E513" t="inlineStr"/>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E513" t="n">
+        <v>0</v>
+      </c>
       <c r="F513" t="inlineStr"/>
       <c r="G513" t="inlineStr"/>
       <c r="H513" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I513" t="inlineStr">
@@ -20326,10 +20388,10 @@
         </is>
       </c>
       <c r="J513" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K513" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="514">
@@ -20348,13 +20410,19 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D514" t="inlineStr"/>
-      <c r="E514" t="inlineStr"/>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E514" t="n">
+        <v>0</v>
+      </c>
       <c r="F514" t="inlineStr"/>
       <c r="G514" t="inlineStr"/>
       <c r="H514" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I514" t="inlineStr">
@@ -20363,10 +20431,10 @@
         </is>
       </c>
       <c r="J514" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K514" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="515">
@@ -20385,13 +20453,19 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D515" t="inlineStr"/>
-      <c r="E515" t="inlineStr"/>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E515" t="n">
+        <v>0</v>
+      </c>
       <c r="F515" t="inlineStr"/>
       <c r="G515" t="inlineStr"/>
       <c r="H515" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I515" t="inlineStr">
@@ -20400,10 +20474,10 @@
         </is>
       </c>
       <c r="J515" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K515" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="516">
@@ -20422,13 +20496,19 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D516" t="inlineStr"/>
-      <c r="E516" t="inlineStr"/>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
+      </c>
+      <c r="E516" t="n">
+        <v>0</v>
+      </c>
       <c r="F516" t="inlineStr"/>
       <c r="G516" t="inlineStr"/>
       <c r="H516" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I516" t="inlineStr">
@@ -20437,10 +20517,10 @@
         </is>
       </c>
       <c r="J516" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K516" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="517">
@@ -20451,7 +20531,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
@@ -20459,13 +20539,17 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D517" t="inlineStr"/>
-      <c r="E517" t="inlineStr"/>
+      <c r="D517" t="n">
+        <v>-22.34110561274889</v>
+      </c>
+      <c r="E517" t="n">
+        <v>1.880219793050742e-40</v>
+      </c>
       <c r="F517" t="inlineStr"/>
       <c r="G517" t="inlineStr"/>
       <c r="H517" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I517" t="inlineStr">
@@ -20474,10 +20558,10 @@
         </is>
       </c>
       <c r="J517" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K517" t="n">
-        <v>0</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="518">
@@ -20488,7 +20572,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
@@ -20497,10 +20581,10 @@
         </is>
       </c>
       <c r="D518" t="n">
-        <v>-22.34110561274889</v>
+        <v>-19.88471453556187</v>
       </c>
       <c r="E518" t="n">
-        <v>1.880219793050742e-40</v>
+        <v>2.38480654894213e-36</v>
       </c>
       <c r="F518" t="inlineStr"/>
       <c r="G518" t="inlineStr"/>
@@ -20515,10 +20599,10 @@
         </is>
       </c>
       <c r="J518" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K518" t="n">
-        <v>2.2</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="519">
@@ -20529,7 +20613,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="C519" t="inlineStr">
@@ -20537,11 +20621,13 @@
           <t>gsm8k</t>
         </is>
       </c>
-      <c r="D519" t="n">
-        <v>-19.88471453556187</v>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>-inf</t>
+        </is>
       </c>
       <c r="E519" t="n">
-        <v>2.38480654894213e-36</v>
+        <v>0</v>
       </c>
       <c r="F519" t="inlineStr"/>
       <c r="G519" t="inlineStr"/>
@@ -20556,10 +20642,10 @@
         </is>
       </c>
       <c r="J519" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K519" t="n">
-        <v>5.11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="520">
@@ -26739,10 +26825,10 @@
         </is>
       </c>
       <c r="D674" t="n">
-        <v>-1.104813744104458</v>
+        <v>-1.162755347846276</v>
       </c>
       <c r="E674" t="n">
-        <v>0.27191819299695</v>
+        <v>0.2477239472782931</v>
       </c>
       <c r="F674" t="inlineStr"/>
       <c r="G674" t="inlineStr"/>
@@ -26757,10 +26843,10 @@
         </is>
       </c>
       <c r="J674" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K674" t="n">
-        <v>23.32084072897347</v>
+        <v>19.75593863231711</v>
       </c>
     </row>
     <row r="675">
@@ -26780,10 +26866,10 @@
         </is>
       </c>
       <c r="D675" t="n">
-        <v>1.052503306293758</v>
+        <v>1.000981683230616</v>
       </c>
       <c r="E675" t="n">
-        <v>0.2951308631083701</v>
+        <v>0.3192760182593382</v>
       </c>
       <c r="F675" t="inlineStr"/>
       <c r="G675" t="inlineStr"/>
@@ -26798,10 +26884,10 @@
         </is>
       </c>
       <c r="J675" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K675" t="n">
-        <v>22.05413470835337</v>
+        <v>18.64404283313305</v>
       </c>
     </row>
     <row r="676">
@@ -26821,10 +26907,10 @@
         </is>
       </c>
       <c r="D676" t="n">
-        <v>3.979465408835954</v>
+        <v>4.075656134833133</v>
       </c>
       <c r="E676" t="n">
-        <v>0.0001317090985153442</v>
+        <v>9.271067799268673e-05</v>
       </c>
       <c r="F676" t="inlineStr"/>
       <c r="G676" t="inlineStr"/>
@@ -26839,10 +26925,10 @@
         </is>
       </c>
       <c r="J676" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K676" t="n">
-        <v>20.94775786743356</v>
+        <v>17.60693821580896</v>
       </c>
     </row>
     <row r="677">
@@ -26862,10 +26948,10 @@
         </is>
       </c>
       <c r="D677" t="n">
-        <v>3.705529981968572</v>
+        <v>3.814566083104667</v>
       </c>
       <c r="E677" t="n">
-        <v>0.0003476474918970133</v>
+        <v>0.0002374970308874316</v>
       </c>
       <c r="F677" t="inlineStr"/>
       <c r="G677" t="inlineStr"/>
@@ -26880,10 +26966,10 @@
         </is>
       </c>
       <c r="J677" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K677" t="n">
-        <v>21.15967533120474</v>
+        <v>17.80247921033215</v>
       </c>
     </row>
     <row r="678">
@@ -26903,10 +26989,10 @@
         </is>
       </c>
       <c r="D678" t="n">
-        <v>3.363496410695966</v>
+        <v>3.715197679247885</v>
       </c>
       <c r="E678" t="n">
-        <v>0.001095596013285775</v>
+        <v>0.0003361955128525203</v>
       </c>
       <c r="F678" t="inlineStr"/>
       <c r="G678" t="inlineStr"/>
@@ -26921,10 +27007,10 @@
         </is>
       </c>
       <c r="J678" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K678" t="n">
-        <v>21.30110606060606</v>
+        <v>17.8461647935398</v>
       </c>
     </row>
     <row r="679">
@@ -26944,10 +27030,10 @@
         </is>
       </c>
       <c r="D679" t="n">
-        <v>3.321373578099958</v>
+        <v>5.374383349862685</v>
       </c>
       <c r="E679" t="n">
-        <v>0.001255498983138217</v>
+        <v>5.116438987720422e-07</v>
       </c>
       <c r="F679" t="inlineStr"/>
       <c r="G679" t="inlineStr"/>
@@ -26962,10 +27048,10 @@
         </is>
       </c>
       <c r="J679" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K679" t="n">
-        <v>21.35750809438882</v>
+        <v>17.37580946488632</v>
       </c>
     </row>
     <row r="680">
@@ -26985,10 +27071,10 @@
         </is>
       </c>
       <c r="D680" t="n">
-        <v>-5.417265966046467</v>
+        <v>-4.683987804542023</v>
       </c>
       <c r="E680" t="n">
-        <v>4.254504644815754e-07</v>
+        <v>8.97087602753729e-06</v>
       </c>
       <c r="F680" t="inlineStr"/>
       <c r="G680" t="inlineStr"/>
@@ -27003,10 +27089,10 @@
         </is>
       </c>
       <c r="J680" t="n">
-        <v>22.61366765260883</v>
+        <v>19.1058669794258</v>
       </c>
       <c r="K680" t="n">
-        <v>24.865331526878</v>
+        <v>20.78059743471588</v>
       </c>
     </row>
     <row r="681">
@@ -27257,10 +27343,10 @@
         </is>
       </c>
       <c r="D688" t="n">
-        <v>0.2257952192652755</v>
+        <v>0.8284450201026073</v>
       </c>
       <c r="E688" t="n">
-        <v>0.8218261834386439</v>
+        <v>0.4094113132586084</v>
       </c>
       <c r="F688" t="inlineStr"/>
       <c r="G688" t="inlineStr"/>
@@ -27275,10 +27361,10 @@
         </is>
       </c>
       <c r="J688" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K688" t="n">
-        <v>18.25889344427502</v>
+        <v>16.08325531778164</v>
       </c>
     </row>
     <row r="689">
@@ -27298,10 +27384,10 @@
         </is>
       </c>
       <c r="D689" t="n">
-        <v>0.4024892677367463</v>
+        <v>0.5868329320228426</v>
       </c>
       <c r="E689" t="n">
-        <v>0.6881917346824865</v>
+        <v>0.5586517602819621</v>
       </c>
       <c r="F689" t="inlineStr"/>
       <c r="G689" t="inlineStr"/>
@@ -27316,10 +27402,10 @@
         </is>
       </c>
       <c r="J689" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K689" t="n">
-        <v>18.22262767787768</v>
+        <v>16.23610026085026</v>
       </c>
     </row>
     <row r="690">
@@ -27339,10 +27425,10 @@
         </is>
       </c>
       <c r="D690" t="n">
-        <v>11.75759143671778</v>
+        <v>12.59556417385856</v>
       </c>
       <c r="E690" t="n">
-        <v>1.695618504130053e-20</v>
+        <v>2.778272270383118e-22</v>
       </c>
       <c r="F690" t="inlineStr"/>
       <c r="G690" t="inlineStr"/>
@@ -27357,10 +27443,10 @@
         </is>
       </c>
       <c r="J690" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K690" t="n">
-        <v>15.05542068335898</v>
+        <v>13.14014422181743</v>
       </c>
     </row>
     <row r="691">
@@ -27380,10 +27466,10 @@
         </is>
       </c>
       <c r="D691" t="n">
-        <v>6.911007442088759</v>
+        <v>7.176600317236545</v>
       </c>
       <c r="E691" t="n">
-        <v>4.729892138221952e-10</v>
+        <v>1.328436419963163e-10</v>
       </c>
       <c r="F691" t="inlineStr"/>
       <c r="G691" t="inlineStr"/>
@@ -27398,10 +27484,10 @@
         </is>
       </c>
       <c r="J691" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K691" t="n">
-        <v>16.25559161517018</v>
+        <v>14.40215772406988</v>
       </c>
     </row>
     <row r="692">
@@ -27421,10 +27507,10 @@
         </is>
       </c>
       <c r="D692" t="n">
-        <v>5.817852016961354</v>
+        <v>5.828661989369855</v>
       </c>
       <c r="E692" t="n">
-        <v>7.347082369133956e-08</v>
+        <v>7.001515597858814e-08</v>
       </c>
       <c r="F692" t="inlineStr"/>
       <c r="G692" t="inlineStr"/>
@@ -27439,10 +27525,10 @@
         </is>
       </c>
       <c r="J692" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K692" t="n">
-        <v>16.43485019739574</v>
+        <v>14.62677465718387</v>
       </c>
     </row>
     <row r="693">
@@ -27462,10 +27548,10 @@
         </is>
       </c>
       <c r="D693" t="n">
-        <v>-7.839615469759146</v>
+        <v>-7.429772102273158</v>
       </c>
       <c r="E693" t="n">
-        <v>5.285455121601761e-12</v>
+        <v>3.910630755608332e-11</v>
       </c>
       <c r="F693" t="inlineStr"/>
       <c r="G693" t="inlineStr"/>
@@ -27480,10 +27566,10 @@
         </is>
       </c>
       <c r="J693" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K693" t="n">
-        <v>21.21212740290674</v>
+        <v>18.94168966869237</v>
       </c>
     </row>
     <row r="694">
@@ -27503,10 +27589,10 @@
         </is>
       </c>
       <c r="D694" t="n">
-        <v>2.014844489108059</v>
+        <v>2.738351571805377</v>
       </c>
       <c r="E694" t="n">
-        <v>0.04663257124271412</v>
+        <v>0.007323064869412894</v>
       </c>
       <c r="F694" t="inlineStr"/>
       <c r="G694" t="inlineStr"/>
@@ -27521,10 +27607,10 @@
         </is>
       </c>
       <c r="J694" t="n">
-        <v>18.35672871572872</v>
+        <v>16.4133777056277</v>
       </c>
       <c r="K694" t="n">
-        <v>17.52684221334221</v>
+        <v>15.37562427849928</v>
       </c>
     </row>
     <row r="695">
@@ -27775,10 +27861,10 @@
         </is>
       </c>
       <c r="D702" t="n">
-        <v>-22.34317810827821</v>
+        <v>-38.28897129671242</v>
       </c>
       <c r="E702" t="n">
-        <v>1.865837799169632e-40</v>
+        <v>3.730656685490866e-61</v>
       </c>
       <c r="F702" t="inlineStr"/>
       <c r="G702" t="inlineStr"/>
@@ -27793,10 +27879,10 @@
         </is>
       </c>
       <c r="J702" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K702" t="n">
-        <v>13.342</v>
+        <v>10.39633333333333</v>
       </c>
     </row>
     <row r="703">
@@ -27816,10 +27902,10 @@
         </is>
       </c>
       <c r="D703" t="n">
-        <v>-46.43675325856265</v>
+        <v>-55.54386537479321</v>
       </c>
       <c r="E703" t="n">
-        <v>5.154865415126227e-69</v>
+        <v>1.975629380725334e-76</v>
       </c>
       <c r="F703" t="inlineStr"/>
       <c r="G703" t="inlineStr"/>
@@ -27834,10 +27920,10 @@
         </is>
       </c>
       <c r="J703" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K703" t="n">
-        <v>18.28528528528529</v>
+        <v>15.46774774774775</v>
       </c>
     </row>
     <row r="704">
@@ -27857,10 +27943,10 @@
         </is>
       </c>
       <c r="D704" t="n">
-        <v>-43.69141151362562</v>
+        <v>-53.45208403293174</v>
       </c>
       <c r="E704" t="n">
-        <v>1.627680697316523e-66</v>
+        <v>7.824118341761889e-75</v>
       </c>
       <c r="F704" t="inlineStr"/>
       <c r="G704" t="inlineStr"/>
@@ -27875,10 +27961,10 @@
         </is>
       </c>
       <c r="J704" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K704" t="n">
-        <v>17.90147899159664</v>
+        <v>15.18010924369748</v>
       </c>
     </row>
     <row r="705">
@@ -27898,10 +27984,10 @@
         </is>
       </c>
       <c r="D705" t="n">
-        <v>-38.72545208980559</v>
+        <v>-49.14462767237107</v>
       </c>
       <c r="E705" t="n">
-        <v>1.302057520086244e-61</v>
+        <v>2.375590899694243e-71</v>
       </c>
       <c r="F705" t="inlineStr"/>
       <c r="G705" t="inlineStr"/>
@@ -27916,10 +28002,10 @@
         </is>
       </c>
       <c r="J705" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K705" t="n">
-        <v>17.11513227513228</v>
+        <v>14.47489417989418</v>
       </c>
     </row>
     <row r="706">
@@ -27939,10 +28025,10 @@
         </is>
       </c>
       <c r="D706" t="n">
-        <v>-25.9755287937918</v>
+        <v>-28.14743989487769</v>
       </c>
       <c r="E706" t="n">
-        <v>5.382013910054717e-46</v>
+        <v>4.856666438921173e-49</v>
       </c>
       <c r="F706" t="inlineStr"/>
       <c r="G706" t="inlineStr"/>
@@ -27957,10 +28043,10 @@
         </is>
       </c>
       <c r="J706" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K706" t="n">
-        <v>22.78857142857143</v>
+        <v>16.92071428571429</v>
       </c>
     </row>
     <row r="707">
@@ -27980,10 +28066,10 @@
         </is>
       </c>
       <c r="D707" t="n">
-        <v>-99.07442625961049</v>
+        <v>-73.10758486398029</v>
       </c>
       <c r="E707" t="n">
-        <v>7.467472989110106e-101</v>
+        <v>5.808135504918742e-88</v>
       </c>
       <c r="F707" t="inlineStr"/>
       <c r="G707" t="inlineStr"/>
@@ -27998,10 +28084,10 @@
         </is>
       </c>
       <c r="J707" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K707" t="n">
-        <v>20.74901515151516</v>
+        <v>14.77530303030303</v>
       </c>
     </row>
     <row r="708">
@@ -28021,10 +28107,10 @@
         </is>
       </c>
       <c r="D708" t="n">
-        <v>25.46056549255987</v>
+        <v>18.93853448984349</v>
       </c>
       <c r="E708" t="n">
-        <v>3.026138844455713e-45</v>
+        <v>1.100174375782855e-34</v>
       </c>
       <c r="F708" t="inlineStr"/>
       <c r="G708" t="inlineStr"/>
@@ -28039,10 +28125,10 @@
         </is>
       </c>
       <c r="J708" t="n">
-        <v>12.581</v>
+        <v>9.249000000000001</v>
       </c>
       <c r="K708" t="n">
-        <v>11.61466666666667</v>
+        <v>8.722999999999999</v>
       </c>
     </row>
     <row r="709">
@@ -28293,10 +28379,10 @@
         </is>
       </c>
       <c r="D716" t="n">
-        <v>-38.00049227878211</v>
+        <v>-42.53540961400277</v>
       </c>
       <c r="E716" t="n">
-        <v>7.523813471566928e-61</v>
+        <v>2.026425181306664e-65</v>
       </c>
       <c r="F716" t="inlineStr"/>
       <c r="G716" t="inlineStr"/>
@@ -28311,10 +28397,10 @@
         </is>
       </c>
       <c r="J716" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K716" t="n">
-        <v>11.26733333333333</v>
+        <v>9.894333333333332</v>
       </c>
     </row>
     <row r="717">
@@ -28334,10 +28420,10 @@
         </is>
       </c>
       <c r="D717" t="n">
-        <v>-27.75883887374171</v>
+        <v>-24.3905475777081</v>
       </c>
       <c r="E717" t="n">
-        <v>1.650082730703056e-48</v>
+        <v>1.189933294707286e-43</v>
       </c>
       <c r="F717" t="inlineStr"/>
       <c r="G717" t="inlineStr"/>
@@ -28352,10 +28438,10 @@
         </is>
       </c>
       <c r="J717" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K717" t="n">
-        <v>13.55895294117647</v>
+        <v>11.49540392156863</v>
       </c>
     </row>
     <row r="718">
@@ -28375,10 +28461,10 @@
         </is>
       </c>
       <c r="D718" t="n">
-        <v>-28.05897048788013</v>
+        <v>-25.35080814542259</v>
       </c>
       <c r="E718" t="n">
-        <v>6.408561315206937e-49</v>
+        <v>4.387109857418391e-45</v>
       </c>
       <c r="F718" t="inlineStr"/>
       <c r="G718" t="inlineStr"/>
@@ -28393,10 +28479,10 @@
         </is>
       </c>
       <c r="J718" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K718" t="n">
-        <v>13.56397317298797</v>
+        <v>11.58013876040703</v>
       </c>
     </row>
     <row r="719">
@@ -28416,10 +28502,10 @@
         </is>
       </c>
       <c r="D719" t="n">
-        <v>-30.64498494098692</v>
+        <v>-27.45012451731748</v>
       </c>
       <c r="E719" t="n">
-        <v>2.535866664593968e-52</v>
+        <v>4.401517005285405e-48</v>
       </c>
       <c r="F719" t="inlineStr"/>
       <c r="G719" t="inlineStr"/>
@@ -28434,10 +28520,10 @@
         </is>
       </c>
       <c r="J719" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K719" t="n">
-        <v>13.72882352941177</v>
+        <v>11.69336974789916</v>
       </c>
     </row>
     <row r="720">
@@ -28457,10 +28543,10 @@
         </is>
       </c>
       <c r="D720" t="n">
-        <v>-28.5688974062822</v>
+        <v>-28.09622079218814</v>
       </c>
       <c r="E720" t="n">
-        <v>1.308249919211199e-49</v>
+        <v>5.701910080054459e-49</v>
       </c>
       <c r="F720" t="inlineStr"/>
       <c r="G720" t="inlineStr"/>
@@ -28475,10 +28561,10 @@
         </is>
       </c>
       <c r="J720" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K720" t="n">
-        <v>13.54330627705628</v>
+        <v>11.66401875901876</v>
       </c>
     </row>
     <row r="721">
@@ -28498,10 +28584,10 @@
         </is>
       </c>
       <c r="D721" t="n">
-        <v>-53.57732691645629</v>
+        <v>-49.08641141363293</v>
       </c>
       <c r="E721" t="n">
-        <v>6.25375474721328e-75</v>
+        <v>2.659159496260932e-71</v>
       </c>
       <c r="F721" t="inlineStr"/>
       <c r="G721" t="inlineStr"/>
@@ -28516,10 +28602,10 @@
         </is>
       </c>
       <c r="J721" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K721" t="n">
-        <v>14.65551282051282</v>
+        <v>12.5599358974359</v>
       </c>
     </row>
     <row r="722">
@@ -28539,10 +28625,10 @@
         </is>
       </c>
       <c r="D722" t="n">
-        <v>17.40454967153083</v>
+        <v>15.72065397270649</v>
       </c>
       <c r="E722" t="n">
-        <v>6.952754269250642e-32</v>
+        <v>1.162833054748654e-28</v>
       </c>
       <c r="F722" t="inlineStr"/>
       <c r="G722" t="inlineStr"/>
@@ -28557,10 +28643,10 @@
         </is>
       </c>
       <c r="J722" t="n">
-        <v>10.095</v>
+        <v>8.647499999999999</v>
       </c>
       <c r="K722" t="n">
-        <v>9.593999999999999</v>
+        <v>8.221</v>
       </c>
     </row>
     <row r="723">

</xml_diff>